<commit_message>
Fixed General values to test diferent solution
</commit_message>
<xml_diff>
--- a/Proyecto/data/horariosProhibidos.xlsx
+++ b/Proyecto/data/horariosProhibidos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UVG\Final Round\Tesis\Prubeas\Git\TG2018\Proyecto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8596E9D5-7983-427B-B108-B992E058E3A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516922B7-E0CE-434A-8733-83EA99B1B2D2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{0392F579-CCC5-450F-A7DF-34F18D5CE9DB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{0392F579-CCC5-450F-A7DF-34F18D5CE9DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Año1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="12">
   <si>
     <t>No. Per.</t>
   </si>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CDE845-13B8-4F9B-A180-E820E1E5BBC8}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +740,9 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -753,10 +755,16 @@
         <v>0.3576388888888889</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -769,10 +777,16 @@
         <v>0.3923611111111111</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -788,7 +802,9 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -820,7 +836,9 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -834,9 +852,13 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -850,9 +872,13 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -868,7 +894,9 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1008,21 +1036,11 @@
       <c r="C22" s="6">
         <v>0.88541666666666663</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1042,7 +1060,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F13"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,13 +1137,15 @@
       <c r="C5" s="3">
         <v>0.32291666666666669</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -1137,13 +1157,15 @@
       <c r="C6" s="3">
         <v>0.3576388888888889</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1157,11 +1179,11 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1193,7 +1215,9 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
@@ -1209,9 +1233,7 @@
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
@@ -1227,9 +1249,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
@@ -1243,13 +1263,17 @@
       <c r="C12" s="3">
         <v>0.54513888888888895</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1261,13 +1285,17 @@
       <c r="C13" s="3">
         <v>0.57986111111111105</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1429,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89261780-7AFC-40F4-B789-99348F02882E}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,9 +1538,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1528,9 +1554,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1546,9 +1570,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1564,9 +1586,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1598,9 +1618,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1616,9 +1634,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1631,13 +1647,15 @@
       <c r="C12" s="3">
         <v>0.54513888888888895</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -1649,13 +1667,15 @@
       <c r="C13" s="3">
         <v>0.57986111111111105</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1667,11 +1687,15 @@
       <c r="C14" s="3">
         <v>0.61458333333333337</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1685,7 +1709,9 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
@@ -1701,7 +1727,9 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
@@ -1748,9 +1776,13 @@
         <v>0.78819444444444453</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1764,9 +1796,13 @@
         <v>0.82291666666666663</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1780,9 +1816,13 @@
         <v>0.85763888888888884</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>